<commit_message>
fixed ehader styles final
</commit_message>
<xml_diff>
--- a/generated_timesheets/December_2025_Timesheet_Shamik_Guha_Ray.xlsx
+++ b/generated_timesheets/December_2025_Timesheet_Shamik_Guha_Ray.xlsx
@@ -89,7 +89,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,7 +103,6 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border/>
     <border>
       <bottom style="medium"/>
     </border>
@@ -111,14 +110,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -526,7 +526,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H52"/>
+  <dimension ref="A2:H52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,1108 +534,1133 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="n"/>
-      <c r="B1" s="1" t="n"/>
-      <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
-      <c r="E1" s="1" t="n"/>
-    </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>To engage Agile Co-Development and ICT Professional Services via 19024 bulk tender (PR230941)</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="2" t="n"/>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Month/Year</t>
         </is>
       </c>
-      <c r="E2" s="3" t="inlineStr">
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>December - 2025</t>
         </is>
       </c>
+      <c r="G2" s="3" t="n"/>
+      <c r="H2" s="3" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="1" t="inlineStr">
         <is>
           <t>PO Ref</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>GVT000ECI24000829</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="2" t="n"/>
+      <c r="E3" t="inlineStr">
         <is>
           <t>Contractor</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>PALO IT</t>
         </is>
       </c>
+      <c r="G3" s="3" t="n"/>
+      <c r="H3" s="3" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="1" t="inlineStr">
         <is>
           <t>PO Date</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>1 May 24 - 30 Apr 25</t>
         </is>
       </c>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="2" t="n"/>
+      <c r="F4" s="1" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+      <c r="A6" s="1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B6" s="4" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>Shamik Guha Ray</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" s="3" t="n"/>
+      <c r="E6" s="1" t="inlineStr">
         <is>
           <t>Skill Level</t>
         </is>
       </c>
-      <c r="E6" s="4" t="inlineStr">
+      <c r="F6" s="2" t="inlineStr">
         <is>
           <t>Professional</t>
         </is>
       </c>
+      <c r="G6" s="3" t="n"/>
+      <c r="H6" s="3" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+      <c r="A7" s="1" t="inlineStr">
         <is>
           <t>Role Specialization</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>DevOps Engineer - II</t>
         </is>
       </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n"/>
+      <c r="F7" s="1" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="inlineStr">
+      <c r="A8" s="1" t="inlineStr">
         <is>
           <t>Group/Specialization</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>Consulting</t>
         </is>
       </c>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="3" t="n"/>
+      <c r="F8" s="1" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="inlineStr">
+      <c r="A10" s="4" t="inlineStr">
         <is>
           <t>SN</t>
         </is>
       </c>
-      <c r="B10" s="5" t="inlineStr">
+      <c r="B10" s="4" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="C10" s="6" t="inlineStr">
+      <c r="C10" s="5" t="inlineStr">
         <is>
           <t>At Work</t>
         </is>
       </c>
-      <c r="D10" s="7" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr">
         <is>
           <t>Public Holiday</t>
         </is>
       </c>
-      <c r="E10" s="8" t="inlineStr">
+      <c r="E10" s="7" t="inlineStr">
         <is>
           <t>Sick Leave</t>
         </is>
       </c>
-      <c r="F10" s="5" t="inlineStr">
+      <c r="F10" s="4" t="inlineStr">
         <is>
           <t>Childcare Leave</t>
         </is>
       </c>
-      <c r="G10" s="9" t="inlineStr">
+      <c r="G10" s="8" t="inlineStr">
         <is>
           <t>Annual Leave</t>
         </is>
       </c>
-      <c r="H10" s="5" t="inlineStr">
+      <c r="H10" s="4" t="inlineStr">
         <is>
           <t>Remarks</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="B11" s="10" t="inlineStr">
+      <c r="B11" s="9" t="inlineStr">
         <is>
           <t>01-December-2025</t>
         </is>
       </c>
-      <c r="C11" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D11" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E11" s="11" t="inlineStr"/>
-      <c r="F11" s="11" t="inlineStr"/>
-      <c r="G11" s="11" t="inlineStr"/>
-      <c r="H11" s="13" t="inlineStr">
+      <c r="C11" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D11" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E11" s="10" t="inlineStr"/>
+      <c r="F11" s="10" t="inlineStr"/>
+      <c r="G11" s="10" t="inlineStr"/>
+      <c r="H11" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="B12" s="10" t="inlineStr">
+      <c r="B12" s="9" t="inlineStr">
         <is>
           <t>02-December-2025</t>
         </is>
       </c>
-      <c r="C12" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D12" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E12" s="11" t="inlineStr"/>
-      <c r="F12" s="11" t="inlineStr"/>
-      <c r="G12" s="11" t="inlineStr"/>
-      <c r="H12" s="13" t="inlineStr">
+      <c r="C12" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D12" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="inlineStr"/>
+      <c r="F12" s="10" t="inlineStr"/>
+      <c r="G12" s="10" t="inlineStr"/>
+      <c r="H12" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="B13" s="10" t="inlineStr">
+      <c r="B13" s="9" t="inlineStr">
         <is>
           <t>03-December-2025</t>
         </is>
       </c>
-      <c r="C13" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D13" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E13" s="11" t="inlineStr"/>
-      <c r="F13" s="11" t="inlineStr"/>
-      <c r="G13" s="11" t="inlineStr"/>
-      <c r="H13" s="13" t="inlineStr">
+      <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D13" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E13" s="10" t="inlineStr"/>
+      <c r="F13" s="10" t="inlineStr"/>
+      <c r="G13" s="10" t="inlineStr"/>
+      <c r="H13" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="B14" s="10" t="inlineStr">
+      <c r="B14" s="9" t="inlineStr">
         <is>
           <t>04-December-2025</t>
         </is>
       </c>
-      <c r="C14" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D14" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E14" s="11" t="inlineStr"/>
-      <c r="F14" s="11" t="inlineStr"/>
-      <c r="G14" s="11" t="inlineStr"/>
-      <c r="H14" s="13" t="inlineStr">
+      <c r="C14" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D14" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E14" s="10" t="inlineStr"/>
+      <c r="F14" s="10" t="inlineStr"/>
+      <c r="G14" s="10" t="inlineStr"/>
+      <c r="H14" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="10" t="n">
+      <c r="A15" s="9" t="n">
         <v>5</v>
       </c>
-      <c r="B15" s="10" t="inlineStr">
+      <c r="B15" s="9" t="inlineStr">
         <is>
           <t>05-December-2025</t>
         </is>
       </c>
-      <c r="C15" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D15" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E15" s="11" t="inlineStr"/>
-      <c r="F15" s="11" t="inlineStr"/>
-      <c r="G15" s="11" t="inlineStr"/>
-      <c r="H15" s="13" t="inlineStr">
+      <c r="C15" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D15" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E15" s="10" t="inlineStr"/>
+      <c r="F15" s="10" t="inlineStr"/>
+      <c r="G15" s="10" t="inlineStr"/>
+      <c r="H15" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="9" t="n">
         <v>6</v>
       </c>
-      <c r="B16" s="10" t="inlineStr">
+      <c r="B16" s="9" t="inlineStr">
         <is>
           <t>06-December-2025</t>
         </is>
       </c>
-      <c r="C16" s="11" t="inlineStr"/>
-      <c r="D16" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E16" s="11" t="inlineStr"/>
-      <c r="F16" s="11" t="inlineStr"/>
-      <c r="G16" s="11" t="inlineStr"/>
-      <c r="H16" s="14" t="inlineStr">
+      <c r="C16" s="10" t="inlineStr"/>
+      <c r="D16" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E16" s="10" t="inlineStr"/>
+      <c r="F16" s="10" t="inlineStr"/>
+      <c r="G16" s="10" t="inlineStr"/>
+      <c r="H16" s="13" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="9" t="n">
         <v>7</v>
       </c>
-      <c r="B17" s="10" t="inlineStr">
+      <c r="B17" s="9" t="inlineStr">
         <is>
           <t>07-December-2025</t>
         </is>
       </c>
-      <c r="C17" s="11" t="inlineStr"/>
-      <c r="D17" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E17" s="11" t="inlineStr"/>
-      <c r="F17" s="11" t="inlineStr"/>
-      <c r="G17" s="11" t="inlineStr"/>
-      <c r="H17" s="14" t="inlineStr">
+      <c r="C17" s="10" t="inlineStr"/>
+      <c r="D17" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E17" s="10" t="inlineStr"/>
+      <c r="F17" s="10" t="inlineStr"/>
+      <c r="G17" s="10" t="inlineStr"/>
+      <c r="H17" s="13" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="10" t="n">
+      <c r="A18" s="9" t="n">
         <v>8</v>
       </c>
-      <c r="B18" s="10" t="inlineStr">
+      <c r="B18" s="9" t="inlineStr">
         <is>
           <t>08-December-2025</t>
         </is>
       </c>
-      <c r="C18" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D18" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E18" s="11" t="inlineStr"/>
-      <c r="F18" s="11" t="inlineStr"/>
-      <c r="G18" s="11" t="inlineStr"/>
-      <c r="H18" s="13" t="inlineStr">
+      <c r="C18" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D18" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E18" s="10" t="inlineStr"/>
+      <c r="F18" s="10" t="inlineStr"/>
+      <c r="G18" s="10" t="inlineStr"/>
+      <c r="H18" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="10" t="n">
+      <c r="A19" s="9" t="n">
         <v>9</v>
       </c>
-      <c r="B19" s="10" t="inlineStr">
+      <c r="B19" s="9" t="inlineStr">
         <is>
           <t>09-December-2025</t>
         </is>
       </c>
-      <c r="C19" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D19" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E19" s="11" t="inlineStr"/>
-      <c r="F19" s="11" t="inlineStr"/>
-      <c r="G19" s="11" t="inlineStr"/>
-      <c r="H19" s="13" t="inlineStr">
+      <c r="C19" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D19" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" s="10" t="inlineStr"/>
+      <c r="F19" s="10" t="inlineStr"/>
+      <c r="G19" s="10" t="inlineStr"/>
+      <c r="H19" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="n">
+      <c r="A20" s="9" t="n">
         <v>10</v>
       </c>
-      <c r="B20" s="10" t="inlineStr">
+      <c r="B20" s="9" t="inlineStr">
         <is>
           <t>10-December-2025</t>
         </is>
       </c>
-      <c r="C20" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D20" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E20" s="11" t="inlineStr"/>
-      <c r="F20" s="11" t="inlineStr"/>
-      <c r="G20" s="11" t="inlineStr"/>
-      <c r="H20" s="13" t="inlineStr">
+      <c r="C20" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D20" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" s="10" t="inlineStr"/>
+      <c r="F20" s="10" t="inlineStr"/>
+      <c r="G20" s="10" t="inlineStr"/>
+      <c r="H20" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="n">
+      <c r="A21" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="10" t="inlineStr">
+      <c r="B21" s="9" t="inlineStr">
         <is>
           <t>11-December-2025</t>
         </is>
       </c>
-      <c r="C21" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D21" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E21" s="11" t="inlineStr"/>
-      <c r="F21" s="11" t="inlineStr"/>
-      <c r="G21" s="11" t="inlineStr"/>
-      <c r="H21" s="13" t="inlineStr">
+      <c r="C21" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D21" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="10" t="inlineStr"/>
+      <c r="F21" s="10" t="inlineStr"/>
+      <c r="G21" s="10" t="inlineStr"/>
+      <c r="H21" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="n">
+      <c r="A22" s="9" t="n">
         <v>12</v>
       </c>
-      <c r="B22" s="10" t="inlineStr">
+      <c r="B22" s="9" t="inlineStr">
         <is>
           <t>12-December-2025</t>
         </is>
       </c>
-      <c r="C22" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D22" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E22" s="11" t="inlineStr"/>
-      <c r="F22" s="11" t="inlineStr"/>
-      <c r="G22" s="11" t="inlineStr"/>
-      <c r="H22" s="13" t="inlineStr">
+      <c r="C22" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D22" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E22" s="10" t="inlineStr"/>
+      <c r="F22" s="10" t="inlineStr"/>
+      <c r="G22" s="10" t="inlineStr"/>
+      <c r="H22" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="10" t="n">
+      <c r="A23" s="9" t="n">
         <v>13</v>
       </c>
-      <c r="B23" s="10" t="inlineStr">
+      <c r="B23" s="9" t="inlineStr">
         <is>
           <t>13-December-2025</t>
         </is>
       </c>
-      <c r="C23" s="11" t="inlineStr"/>
-      <c r="D23" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E23" s="11" t="inlineStr"/>
-      <c r="F23" s="11" t="inlineStr"/>
-      <c r="G23" s="11" t="inlineStr"/>
-      <c r="H23" s="14" t="inlineStr">
+      <c r="C23" s="10" t="inlineStr"/>
+      <c r="D23" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E23" s="10" t="inlineStr"/>
+      <c r="F23" s="10" t="inlineStr"/>
+      <c r="G23" s="10" t="inlineStr"/>
+      <c r="H23" s="13" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="10" t="n">
+      <c r="A24" s="9" t="n">
         <v>14</v>
       </c>
-      <c r="B24" s="10" t="inlineStr">
+      <c r="B24" s="9" t="inlineStr">
         <is>
           <t>14-December-2025</t>
         </is>
       </c>
-      <c r="C24" s="11" t="inlineStr"/>
-      <c r="D24" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E24" s="11" t="inlineStr"/>
-      <c r="F24" s="11" t="inlineStr"/>
-      <c r="G24" s="11" t="inlineStr"/>
-      <c r="H24" s="14" t="inlineStr">
+      <c r="C24" s="10" t="inlineStr"/>
+      <c r="D24" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" s="10" t="inlineStr"/>
+      <c r="F24" s="10" t="inlineStr"/>
+      <c r="G24" s="10" t="inlineStr"/>
+      <c r="H24" s="13" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="10" t="n">
+      <c r="A25" s="9" t="n">
         <v>15</v>
       </c>
-      <c r="B25" s="10" t="inlineStr">
+      <c r="B25" s="9" t="inlineStr">
         <is>
           <t>15-December-2025</t>
         </is>
       </c>
-      <c r="C25" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D25" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E25" s="11" t="inlineStr"/>
-      <c r="F25" s="11" t="inlineStr"/>
-      <c r="G25" s="11" t="inlineStr"/>
-      <c r="H25" s="13" t="inlineStr">
+      <c r="C25" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D25" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" s="10" t="inlineStr"/>
+      <c r="F25" s="10" t="inlineStr"/>
+      <c r="G25" s="10" t="inlineStr"/>
+      <c r="H25" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="10" t="n">
+      <c r="A26" s="9" t="n">
         <v>16</v>
       </c>
-      <c r="B26" s="10" t="inlineStr">
+      <c r="B26" s="9" t="inlineStr">
         <is>
           <t>16-December-2025</t>
         </is>
       </c>
-      <c r="C26" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D26" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E26" s="11" t="inlineStr"/>
-      <c r="F26" s="11" t="inlineStr"/>
-      <c r="G26" s="11" t="inlineStr"/>
-      <c r="H26" s="13" t="inlineStr">
+      <c r="C26" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D26" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" s="10" t="inlineStr"/>
+      <c r="F26" s="10" t="inlineStr"/>
+      <c r="G26" s="10" t="inlineStr"/>
+      <c r="H26" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="10" t="n">
+      <c r="A27" s="9" t="n">
         <v>17</v>
       </c>
-      <c r="B27" s="10" t="inlineStr">
+      <c r="B27" s="9" t="inlineStr">
         <is>
           <t>17-December-2025</t>
         </is>
       </c>
-      <c r="C27" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D27" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E27" s="11" t="inlineStr"/>
-      <c r="F27" s="11" t="inlineStr"/>
-      <c r="G27" s="11" t="inlineStr"/>
-      <c r="H27" s="13" t="inlineStr">
+      <c r="C27" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D27" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E27" s="10" t="inlineStr"/>
+      <c r="F27" s="10" t="inlineStr"/>
+      <c r="G27" s="10" t="inlineStr"/>
+      <c r="H27" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="10" t="n">
+      <c r="A28" s="9" t="n">
         <v>18</v>
       </c>
-      <c r="B28" s="10" t="inlineStr">
+      <c r="B28" s="9" t="inlineStr">
         <is>
           <t>18-December-2025</t>
         </is>
       </c>
-      <c r="C28" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D28" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E28" s="11" t="inlineStr"/>
-      <c r="F28" s="11" t="inlineStr"/>
-      <c r="G28" s="11" t="inlineStr"/>
-      <c r="H28" s="13" t="inlineStr">
+      <c r="C28" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D28" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" s="10" t="inlineStr"/>
+      <c r="F28" s="10" t="inlineStr"/>
+      <c r="G28" s="10" t="inlineStr"/>
+      <c r="H28" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="10" t="n">
+      <c r="A29" s="9" t="n">
         <v>19</v>
       </c>
-      <c r="B29" s="10" t="inlineStr">
+      <c r="B29" s="9" t="inlineStr">
         <is>
           <t>19-December-2025</t>
         </is>
       </c>
-      <c r="C29" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D29" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E29" s="11" t="inlineStr"/>
-      <c r="F29" s="11" t="inlineStr"/>
-      <c r="G29" s="11" t="inlineStr"/>
-      <c r="H29" s="13" t="inlineStr">
+      <c r="C29" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D29" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" s="10" t="inlineStr"/>
+      <c r="F29" s="10" t="inlineStr"/>
+      <c r="G29" s="10" t="inlineStr"/>
+      <c r="H29" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="10" t="n">
+      <c r="A30" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="B30" s="10" t="inlineStr">
+      <c r="B30" s="9" t="inlineStr">
         <is>
           <t>20-December-2025</t>
         </is>
       </c>
-      <c r="C30" s="11" t="inlineStr"/>
-      <c r="D30" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E30" s="11" t="inlineStr"/>
-      <c r="F30" s="11" t="inlineStr"/>
-      <c r="G30" s="11" t="inlineStr"/>
-      <c r="H30" s="14" t="inlineStr">
+      <c r="C30" s="10" t="inlineStr"/>
+      <c r="D30" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E30" s="10" t="inlineStr"/>
+      <c r="F30" s="10" t="inlineStr"/>
+      <c r="G30" s="10" t="inlineStr"/>
+      <c r="H30" s="13" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="10" t="n">
+      <c r="A31" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="B31" s="10" t="inlineStr">
+      <c r="B31" s="9" t="inlineStr">
         <is>
           <t>21-December-2025</t>
         </is>
       </c>
-      <c r="C31" s="11" t="inlineStr"/>
-      <c r="D31" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E31" s="11" t="inlineStr"/>
-      <c r="F31" s="11" t="inlineStr"/>
-      <c r="G31" s="11" t="inlineStr"/>
-      <c r="H31" s="14" t="inlineStr">
+      <c r="C31" s="10" t="inlineStr"/>
+      <c r="D31" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" s="10" t="inlineStr"/>
+      <c r="F31" s="10" t="inlineStr"/>
+      <c r="G31" s="10" t="inlineStr"/>
+      <c r="H31" s="13" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="10" t="n">
+      <c r="A32" s="9" t="n">
         <v>22</v>
       </c>
-      <c r="B32" s="10" t="inlineStr">
+      <c r="B32" s="9" t="inlineStr">
         <is>
           <t>22-December-2025</t>
         </is>
       </c>
-      <c r="C32" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D32" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E32" s="11" t="inlineStr"/>
-      <c r="F32" s="11" t="inlineStr"/>
-      <c r="G32" s="11" t="inlineStr"/>
-      <c r="H32" s="13" t="inlineStr">
+      <c r="C32" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D32" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" s="10" t="inlineStr"/>
+      <c r="F32" s="10" t="inlineStr"/>
+      <c r="G32" s="10" t="inlineStr"/>
+      <c r="H32" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="10" t="n">
+      <c r="A33" s="9" t="n">
         <v>23</v>
       </c>
-      <c r="B33" s="10" t="inlineStr">
+      <c r="B33" s="9" t="inlineStr">
         <is>
           <t>23-December-2025</t>
         </is>
       </c>
-      <c r="C33" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D33" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E33" s="11" t="inlineStr"/>
-      <c r="F33" s="11" t="inlineStr"/>
-      <c r="G33" s="11" t="inlineStr"/>
-      <c r="H33" s="13" t="inlineStr">
+      <c r="C33" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D33" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" s="10" t="inlineStr"/>
+      <c r="F33" s="10" t="inlineStr"/>
+      <c r="G33" s="10" t="inlineStr"/>
+      <c r="H33" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="10" t="n">
+      <c r="A34" s="9" t="n">
         <v>24</v>
       </c>
-      <c r="B34" s="10" t="inlineStr">
+      <c r="B34" s="9" t="inlineStr">
         <is>
           <t>24-December-2025</t>
         </is>
       </c>
-      <c r="C34" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D34" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E34" s="11" t="inlineStr"/>
-      <c r="F34" s="11" t="inlineStr"/>
-      <c r="G34" s="11" t="inlineStr"/>
-      <c r="H34" s="13" t="inlineStr">
+      <c r="C34" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D34" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" s="10" t="inlineStr"/>
+      <c r="F34" s="10" t="inlineStr"/>
+      <c r="G34" s="10" t="inlineStr"/>
+      <c r="H34" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="10" t="n">
+      <c r="A35" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="B35" s="10" t="inlineStr">
+      <c r="B35" s="9" t="inlineStr">
         <is>
           <t>25-December-2025</t>
         </is>
       </c>
-      <c r="C35" s="11" t="inlineStr"/>
-      <c r="D35" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="E35" s="11" t="inlineStr"/>
-      <c r="F35" s="11" t="inlineStr"/>
-      <c r="G35" s="11" t="inlineStr"/>
-      <c r="H35" s="14" t="inlineStr">
+      <c r="C35" s="10" t="inlineStr"/>
+      <c r="D35" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E35" s="10" t="inlineStr"/>
+      <c r="F35" s="10" t="inlineStr"/>
+      <c r="G35" s="10" t="inlineStr"/>
+      <c r="H35" s="13" t="inlineStr">
         <is>
           <t>Christmas Day</t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="10" t="n">
+      <c r="A36" s="9" t="n">
         <v>26</v>
       </c>
-      <c r="B36" s="10" t="inlineStr">
+      <c r="B36" s="9" t="inlineStr">
         <is>
           <t>26-December-2025</t>
         </is>
       </c>
-      <c r="C36" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D36" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E36" s="11" t="inlineStr"/>
-      <c r="F36" s="11" t="inlineStr"/>
-      <c r="G36" s="11" t="inlineStr"/>
-      <c r="H36" s="13" t="inlineStr">
+      <c r="C36" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D36" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E36" s="10" t="inlineStr"/>
+      <c r="F36" s="10" t="inlineStr"/>
+      <c r="G36" s="10" t="inlineStr"/>
+      <c r="H36" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="10" t="n">
+      <c r="A37" s="9" t="n">
         <v>27</v>
       </c>
-      <c r="B37" s="10" t="inlineStr">
+      <c r="B37" s="9" t="inlineStr">
         <is>
           <t>27-December-2025</t>
         </is>
       </c>
-      <c r="C37" s="11" t="inlineStr"/>
-      <c r="D37" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E37" s="11" t="inlineStr"/>
-      <c r="F37" s="11" t="inlineStr"/>
-      <c r="G37" s="11" t="inlineStr"/>
-      <c r="H37" s="14" t="inlineStr">
+      <c r="C37" s="10" t="inlineStr"/>
+      <c r="D37" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E37" s="10" t="inlineStr"/>
+      <c r="F37" s="10" t="inlineStr"/>
+      <c r="G37" s="10" t="inlineStr"/>
+      <c r="H37" s="13" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="10" t="n">
+      <c r="A38" s="9" t="n">
         <v>28</v>
       </c>
-      <c r="B38" s="10" t="inlineStr">
+      <c r="B38" s="9" t="inlineStr">
         <is>
           <t>28-December-2025</t>
         </is>
       </c>
-      <c r="C38" s="11" t="inlineStr"/>
-      <c r="D38" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E38" s="11" t="inlineStr"/>
-      <c r="F38" s="11" t="inlineStr"/>
-      <c r="G38" s="11" t="inlineStr"/>
-      <c r="H38" s="14" t="inlineStr">
+      <c r="C38" s="10" t="inlineStr"/>
+      <c r="D38" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E38" s="10" t="inlineStr"/>
+      <c r="F38" s="10" t="inlineStr"/>
+      <c r="G38" s="10" t="inlineStr"/>
+      <c r="H38" s="13" t="inlineStr">
         <is>
           <t>Sunday</t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="10" t="n">
+      <c r="A39" s="9" t="n">
         <v>29</v>
       </c>
-      <c r="B39" s="10" t="inlineStr">
+      <c r="B39" s="9" t="inlineStr">
         <is>
           <t>29-December-2025</t>
         </is>
       </c>
-      <c r="C39" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D39" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E39" s="11" t="inlineStr"/>
-      <c r="F39" s="11" t="inlineStr"/>
-      <c r="G39" s="11" t="inlineStr"/>
-      <c r="H39" s="13" t="inlineStr">
+      <c r="C39" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D39" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E39" s="10" t="inlineStr"/>
+      <c r="F39" s="10" t="inlineStr"/>
+      <c r="G39" s="10" t="inlineStr"/>
+      <c r="H39" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="10" t="n">
+      <c r="A40" s="9" t="n">
         <v>30</v>
       </c>
-      <c r="B40" s="10" t="inlineStr">
+      <c r="B40" s="9" t="inlineStr">
         <is>
           <t>30-December-2025</t>
         </is>
       </c>
-      <c r="C40" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D40" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E40" s="11" t="inlineStr"/>
-      <c r="F40" s="11" t="inlineStr"/>
-      <c r="G40" s="11" t="inlineStr"/>
-      <c r="H40" s="13" t="inlineStr">
+      <c r="C40" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D40" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E40" s="10" t="inlineStr"/>
+      <c r="F40" s="10" t="inlineStr"/>
+      <c r="G40" s="10" t="inlineStr"/>
+      <c r="H40" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="10" t="n">
+      <c r="A41" s="9" t="n">
         <v>31</v>
       </c>
-      <c r="B41" s="10" t="inlineStr">
+      <c r="B41" s="9" t="inlineStr">
         <is>
           <t>31-December-2025</t>
         </is>
       </c>
-      <c r="C41" s="11" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="D41" s="12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E41" s="11" t="inlineStr"/>
-      <c r="F41" s="11" t="inlineStr"/>
-      <c r="G41" s="11" t="inlineStr"/>
-      <c r="H41" s="13" t="inlineStr">
+      <c r="C41" s="10" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="D41" s="11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E41" s="10" t="inlineStr"/>
+      <c r="F41" s="10" t="inlineStr"/>
+      <c r="G41" s="10" t="inlineStr"/>
+      <c r="H41" s="12" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="H42" s="15" t="n"/>
+      <c r="H42" s="14" t="n"/>
     </row>
     <row r="43">
-      <c r="H43" s="15" t="n"/>
+      <c r="H43" s="14" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="16" t="inlineStr">
+      <c r="A44" s="15" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B44" s="2" t="n"/>
-      <c r="C44" s="17" t="inlineStr">
+      <c r="B44" s="1" t="n"/>
+      <c r="C44" s="16" t="inlineStr">
         <is>
           <t>22.0</t>
         </is>
       </c>
-      <c r="D44" s="17" t="inlineStr">
-        <is>
-          <t>1.0</t>
-        </is>
-      </c>
-      <c r="E44" s="17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="F44" s="17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G44" s="17" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="H44" s="18" t="n"/>
+      <c r="D44" s="16" t="inlineStr">
+        <is>
+          <t>1.0</t>
+        </is>
+      </c>
+      <c r="E44" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F44" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" s="16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H44" s="17" t="n"/>
     </row>
     <row r="45">
-      <c r="H45" s="15" t="n"/>
+      <c r="H45" s="14" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="inlineStr">
+      <c r="A46" s="1" t="inlineStr">
         <is>
           <t>Officer</t>
         </is>
       </c>
-      <c r="B46" s="10" t="inlineStr">
+      <c r="B46" s="9" t="inlineStr">
         <is>
           <t>Shamik Guha Ray</t>
         </is>
       </c>
-      <c r="H46" s="15" t="n"/>
+      <c r="H46" s="14" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="2" t="inlineStr">
+      <c r="A47" s="1" t="inlineStr">
         <is>
           <t>Signature</t>
         </is>
       </c>
-      <c r="B47" s="10" t="inlineStr">
+      <c r="B47" s="9" t="inlineStr">
         <is>
           <t>Shamik Guha Ray</t>
         </is>
       </c>
-      <c r="H47" s="15" t="n"/>
+      <c r="H47" s="14" t="n"/>
     </row>
     <row r="48">
-      <c r="A48" s="2" t="inlineStr">
+      <c r="A48" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B48" s="10" t="inlineStr">
+      <c r="B48" s="9" t="inlineStr">
         <is>
           <t>10 - February - 2025</t>
         </is>
       </c>
-      <c r="H48" s="15" t="n"/>
+      <c r="H48" s="14" t="n"/>
     </row>
     <row r="49">
-      <c r="A49" s="2" t="n"/>
-      <c r="B49" s="2" t="n"/>
-      <c r="H49" s="15" t="n"/>
+      <c r="A49" s="1" t="n"/>
+      <c r="B49" s="1" t="n"/>
+      <c r="H49" s="14" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="2" t="inlineStr">
+      <c r="A50" s="1" t="inlineStr">
         <is>
           <t>Reporting Officer</t>
         </is>
       </c>
-      <c r="B50" s="10" t="inlineStr">
+      <c r="B50" s="9" t="inlineStr">
         <is>
           <t>Deepu Joseph</t>
         </is>
       </c>
-      <c r="H50" s="15" t="n"/>
+      <c r="H50" s="14" t="n"/>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="inlineStr">
+      <c r="A51" s="1" t="inlineStr">
         <is>
           <t>Signature</t>
         </is>
       </c>
-      <c r="B51" s="2" t="inlineStr"/>
-      <c r="H51" s="15" t="n"/>
+      <c r="B51" s="1" t="inlineStr"/>
+      <c r="H51" s="14" t="n"/>
     </row>
     <row r="52">
-      <c r="A52" s="2" t="inlineStr">
+      <c r="A52" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="B52" s="2" t="inlineStr"/>
-      <c r="H52" s="15" t="n"/>
+      <c r="B52" s="1" t="inlineStr"/>
+      <c r="H52" s="14" t="n"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>